<commit_message>
input and valid login added
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -1,19 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{155C1055-8C78-483E-8716-5911FAC4CB4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\B88 Selenium\Workspace\framework\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E481B1B-3118-4C1B-AF9C-B1D753ED5F6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,31 +25,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Akshara</t>
+    <t>Admin</t>
   </si>
   <si>
-    <t>Swara</t>
+    <t>admin123</t>
   </si>
   <si>
-    <t>pink</t>
+    <t>Username</t>
   </si>
   <si>
-    <t>swara</t>
-  </si>
-  <si>
-    <t>bhanu</t>
-  </si>
-  <si>
-    <t>clone</t>
+    <t>Password</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -357,54 +354,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s" s="0">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="0">
+      <c r="B2" t="s">
         <v>1</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>